<commit_message>
Added TSPUC and filled risks table
</commit_message>
<xml_diff>
--- a/Risk Management/Risks.xlsx
+++ b/Risk Management/Risks.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baeuml\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\Semester 3\FitnessWebAppDocumentation\Risk Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CC50426-A05C-4A87-BF96-5B5DEB1BB1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4240268F-44EC-4E50-A009-833AA3F8A2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{40424BBB-2E24-45C8-9705-AAA2AAF021EF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{40424BBB-2E24-45C8-9705-AAA2AAF021EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$G$1:$G$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Risk</t>
   </si>
@@ -55,6 +58,72 @@
   </si>
   <si>
     <t>Risk Factor (sort)</t>
+  </si>
+  <si>
+    <t>Time Management</t>
+  </si>
+  <si>
+    <t>Complexity and Skills</t>
+  </si>
+  <si>
+    <t>Illness</t>
+  </si>
+  <si>
+    <t>Technologies</t>
+  </si>
+  <si>
+    <t>(Bad) Architecture (Refractoring)</t>
+  </si>
+  <si>
+    <t>Loss of Team members</t>
+  </si>
+  <si>
+    <t>Not getting work done due to illness</t>
+  </si>
+  <si>
+    <t>Having missing overview and understanding of the codebase and thus struggeling with tasks</t>
+  </si>
+  <si>
+    <t>Having missing competence with the used technologies and thus strggeling with tasks</t>
+  </si>
+  <si>
+    <t>Someone dropping out and thus loosing a lot of workforce</t>
+  </si>
+  <si>
+    <t>Making bad architectural decisions and thus having to refractor a lot</t>
+  </si>
+  <si>
+    <t>underestimate Issues thus taking way longer than expected</t>
+  </si>
+  <si>
+    <t>Bootcamps and peerprogramming</t>
+  </si>
+  <si>
+    <t>freetime is canceled</t>
+  </si>
+  <si>
+    <t>Don`t be a pussy</t>
+  </si>
+  <si>
+    <t>Team member still has to keep working on the project</t>
+  </si>
+  <si>
+    <t>Can`t be worse than the twin towers</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Johannes</t>
+  </si>
+  <si>
+    <t>Willi</t>
+  </si>
+  <si>
+    <t>Nico</t>
+  </si>
+  <si>
+    <t>Thomas</t>
   </si>
 </sst>
 </file>
@@ -78,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -86,12 +155,134 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -406,47 +597,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9678E7F5-D005-4DF6-BFD0-8501458AE526}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="8">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="2">
+        <f>C2*D2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="D3" s="8">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2">
+        <f>C3*D3</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="8">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="2">
+        <f>C4*D4</f>
+        <v>1.7999999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="8">
+        <v>7</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2">
+        <f>C5*D5</f>
+        <v>0.70000000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="8">
+        <v>10</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="2">
+        <f>C6*D6</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="3">
+        <f>C7*D7</f>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="G1:G7" xr:uid="{9678E7F5-D005-4DF6-BFD0-8501458AE526}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G7">
+      <sortCondition descending="1" ref="G1:G7"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added auto generated class diagram
</commit_message>
<xml_diff>
--- a/Risk Management/Risks.xlsx
+++ b/Risk Management/Risks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\Semester 3\FitnessWebAppDocumentation\Risk Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester 3\FitnessWebAppDocumentation\Risk Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4240268F-44EC-4E50-A009-833AA3F8A2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C83F07-D7B6-44A0-9D82-1F9778B28727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{40424BBB-2E24-45C8-9705-AAA2AAF021EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{40424BBB-2E24-45C8-9705-AAA2AAF021EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -23,15 +23,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -102,15 +93,9 @@
     <t>freetime is canceled</t>
   </si>
   <si>
-    <t>Don`t be a pussy</t>
-  </si>
-  <si>
     <t>Team member still has to keep working on the project</t>
   </si>
   <si>
-    <t>Can`t be worse than the twin towers</t>
-  </si>
-  <si>
     <t>Nick</t>
   </si>
   <si>
@@ -124,6 +109,12 @@
   </si>
   <si>
     <t>Thomas</t>
+  </si>
+  <si>
+    <t>Try shifting the ill persons work to other teammembers</t>
+  </si>
+  <si>
+    <t>When unsure how to build something ask teammembers</t>
   </si>
 </sst>
 </file>
@@ -599,22 +590,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9678E7F5-D005-4DF6-BFD0-8501458AE526}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -637,7 +628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -654,14 +645,14 @@
         <v>19</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2">
-        <f>C2*D2</f>
+        <f t="shared" ref="G2:G7" si="0">C2*D2</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -678,14 +669,14 @@
         <v>20</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2">
-        <f>C3*D3</f>
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -702,14 +693,14 @@
         <v>19</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2">
-        <f>C4*D4</f>
+        <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -723,17 +714,17 @@
         <v>7</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="G5" s="2">
-        <f>C5*D5</f>
+        <f t="shared" si="0"/>
         <v>0.70000000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -747,17 +738,17 @@
         <v>10</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G6" s="2">
-        <f>C6*D6</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -771,13 +762,13 @@
         <v>2</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G7" s="3">
-        <f>C7*D7</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>

</xml_diff>